<commit_message>
docs: update sheets for 2023-06
</commit_message>
<xml_diff>
--- a/汽车收入与开支记录.xlsx
+++ b/汽车收入与开支记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\finance\recording\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8017C6F1-23E8-481D-958F-1A50A307A70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747A4727-BF7E-46C1-BF18-5440517CC59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="285" windowWidth="29040" windowHeight="15615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="300" windowWidth="23256" windowHeight="12348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -627,19 +627,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J37" sqref="J37"/>
+      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="8" width="9" style="2"/>
-    <col min="9" max="9" width="10.5" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.375" style="2"/>
+    <col min="9" max="9" width="10.44140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" style="2"/>
     <col min="11" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -661,7 +661,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
       <c r="B2" s="14"/>
       <c r="C2" s="4" t="s">
@@ -687,7 +687,7 @@
       </c>
       <c r="J2" s="15"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>12</v>
       </c>
@@ -720,7 +720,7 @@
         <v>-732.93000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="21"/>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -751,7 +751,7 @@
         <v>6.2000000000000455</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="21"/>
       <c r="B5" s="1" t="s">
         <v>15</v>
@@ -782,7 +782,7 @@
         <v>-388.07</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
@@ -813,7 +813,7 @@
         <v>-382</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
@@ -844,7 +844,7 @@
         <v>-210</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="1" t="s">
         <v>18</v>
@@ -875,7 +875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>19</v>
       </c>
@@ -908,7 +908,7 @@
         <v>-300</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="1" t="s">
         <v>21</v>
@@ -939,7 +939,7 @@
         <v>-285</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="1" t="s">
         <v>22</v>
@@ -970,7 +970,7 @@
         <v>-1785</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="5" t="s">
         <v>23</v>
@@ -1001,7 +1001,7 @@
         <v>-734.93000000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="B13" s="1" t="s">
         <v>24</v>
@@ -1032,7 +1032,7 @@
         <v>-215.7</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="5" t="s">
         <v>25</v>
@@ -1063,7 +1063,7 @@
         <v>-3986.7400000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="1" t="s">
         <v>13</v>
@@ -1094,7 +1094,7 @@
         <v>-276.89999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
       <c r="B16" s="5" t="s">
         <v>14</v>
@@ -1125,7 +1125,7 @@
         <v>-95.419999999999959</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="1" t="s">
         <v>15</v>
@@ -1156,7 +1156,7 @@
         <v>-278.98</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="21"/>
       <c r="B18" s="5" t="s">
         <v>16</v>
@@ -1187,7 +1187,7 @@
         <v>-11.700000000000045</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
       <c r="B19" s="5" t="s">
         <v>26</v>
@@ -1218,7 +1218,7 @@
         <v>-77.650000000000034</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="5" t="s">
         <v>18</v>
@@ -1249,7 +1249,7 @@
         <v>34.490000000000009</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>27</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>-21.180000000000035</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="5" t="s">
         <v>21</v>
@@ -1313,7 +1313,7 @@
         <v>-221.57</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="5" t="s">
         <v>22</v>
@@ -1344,7 +1344,7 @@
         <v>-59.820000000000022</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="5" t="s">
         <v>23</v>
@@ -1375,7 +1375,7 @@
         <v>-16.080000000000013</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="5" t="s">
         <v>24</v>
@@ -1406,7 +1406,7 @@
         <v>-230</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="5" t="s">
         <v>25</v>
@@ -1437,7 +1437,7 @@
         <v>-3857.52</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="1" t="s">
         <v>13</v>
@@ -1468,7 +1468,7 @@
         <v>-280</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="6" t="s">
         <v>14</v>
@@ -1499,7 +1499,7 @@
         <v>-181.54</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="6" t="s">
         <v>15</v>
@@ -1530,7 +1530,7 @@
         <v>-452.79</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="6" t="s">
         <v>16</v>
@@ -1561,7 +1561,7 @@
         <v>-650.9</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="6" t="s">
         <v>17</v>
@@ -1592,7 +1592,7 @@
         <v>-603.41000000000008</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="6" t="s">
         <v>18</v>
@@ -1623,7 +1623,7 @@
         <v>-894.4</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>28</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>-148</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="6" t="s">
         <v>21</v>
@@ -1687,7 +1687,7 @@
         <v>-2015.5</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="6" t="s">
         <v>22</v>
@@ -1718,7 +1718,7 @@
         <v>-799.4</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="6" t="s">
         <v>23</v>
@@ -1749,7 +1749,7 @@
         <v>-554.84</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="6" t="s">
         <v>24</v>
@@ -1780,43 +1780,68 @@
         <v>-272.39999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C38" s="2">
+        <v>270.39999999999998</v>
+      </c>
+      <c r="D38" s="2">
+        <v>203</v>
+      </c>
+      <c r="E38" s="2">
+        <v>11</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0</v>
+      </c>
+      <c r="G38" s="2">
+        <v>3294.04</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0</v>
+      </c>
+      <c r="I38" s="2">
+        <v>0</v>
+      </c>
+      <c r="J38" s="2">
+        <f>(H38+I38)-(C38+D38+E38+F38+G38)</f>
+        <v>-3778.44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="6" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
docs: update sheets for 2023-07
</commit_message>
<xml_diff>
--- a/汽车收入与开支记录.xlsx
+++ b/汽车收入与开支记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\finance\recording\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747A4727-BF7E-46C1-BF18-5440517CC59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DDECDF-20FE-46F7-8D8B-F83E29D16383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="300" windowWidth="23256" windowHeight="12348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="285" windowWidth="29040" windowHeight="15615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -627,19 +627,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
+      <selection pane="bottomLeft" activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="8" width="9" style="2"/>
-    <col min="9" max="9" width="10.44140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" style="2"/>
+    <col min="9" max="9" width="10.5" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.375" style="2"/>
     <col min="11" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -661,7 +661,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="19"/>
       <c r="B2" s="14"/>
       <c r="C2" s="4" t="s">
@@ -687,7 +687,7 @@
       </c>
       <c r="J2" s="15"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>12</v>
       </c>
@@ -720,7 +720,7 @@
         <v>-732.93000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="21"/>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -751,7 +751,7 @@
         <v>6.2000000000000455</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="21"/>
       <c r="B5" s="1" t="s">
         <v>15</v>
@@ -782,7 +782,7 @@
         <v>-388.07</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="21"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
@@ -813,7 +813,7 @@
         <v>-382</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="21"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
@@ -844,7 +844,7 @@
         <v>-210</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="22"/>
       <c r="B8" s="1" t="s">
         <v>18</v>
@@ -875,7 +875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
         <v>19</v>
       </c>
@@ -908,7 +908,7 @@
         <v>-300</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="21"/>
       <c r="B10" s="1" t="s">
         <v>21</v>
@@ -939,7 +939,7 @@
         <v>-285</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="21"/>
       <c r="B11" s="1" t="s">
         <v>22</v>
@@ -970,7 +970,7 @@
         <v>-1785</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="21"/>
       <c r="B12" s="5" t="s">
         <v>23</v>
@@ -1001,7 +1001,7 @@
         <v>-734.93000000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="21"/>
       <c r="B13" s="1" t="s">
         <v>24</v>
@@ -1032,7 +1032,7 @@
         <v>-215.7</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="21"/>
       <c r="B14" s="5" t="s">
         <v>25</v>
@@ -1063,7 +1063,7 @@
         <v>-3986.7400000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="21"/>
       <c r="B15" s="1" t="s">
         <v>13</v>
@@ -1094,7 +1094,7 @@
         <v>-276.89999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="21"/>
       <c r="B16" s="5" t="s">
         <v>14</v>
@@ -1125,7 +1125,7 @@
         <v>-95.419999999999959</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="21"/>
       <c r="B17" s="1" t="s">
         <v>15</v>
@@ -1156,7 +1156,7 @@
         <v>-278.98</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="21"/>
       <c r="B18" s="5" t="s">
         <v>16</v>
@@ -1187,7 +1187,7 @@
         <v>-11.700000000000045</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="21"/>
       <c r="B19" s="5" t="s">
         <v>26</v>
@@ -1218,7 +1218,7 @@
         <v>-77.650000000000034</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="22"/>
       <c r="B20" s="5" t="s">
         <v>18</v>
@@ -1249,7 +1249,7 @@
         <v>34.490000000000009</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>27</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>-21.180000000000035</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="5" t="s">
         <v>21</v>
@@ -1313,7 +1313,7 @@
         <v>-221.57</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="5" t="s">
         <v>22</v>
@@ -1344,7 +1344,7 @@
         <v>-59.820000000000022</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="5" t="s">
         <v>23</v>
@@ -1375,7 +1375,7 @@
         <v>-16.080000000000013</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
       <c r="B25" s="5" t="s">
         <v>24</v>
@@ -1406,7 +1406,7 @@
         <v>-230</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="5" t="s">
         <v>25</v>
@@ -1437,7 +1437,7 @@
         <v>-3857.52</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
       <c r="B27" s="1" t="s">
         <v>13</v>
@@ -1468,7 +1468,7 @@
         <v>-280</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="6" t="s">
         <v>14</v>
@@ -1499,7 +1499,7 @@
         <v>-181.54</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
       <c r="B29" s="6" t="s">
         <v>15</v>
@@ -1530,7 +1530,7 @@
         <v>-452.79</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="6" t="s">
         <v>16</v>
@@ -1561,7 +1561,7 @@
         <v>-650.9</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
       <c r="B31" s="6" t="s">
         <v>17</v>
@@ -1592,7 +1592,7 @@
         <v>-603.41000000000008</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
       <c r="B32" s="6" t="s">
         <v>18</v>
@@ -1623,7 +1623,7 @@
         <v>-894.4</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>28</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>-148</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
       <c r="B34" s="6" t="s">
         <v>21</v>
@@ -1687,7 +1687,7 @@
         <v>-2015.5</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
       <c r="B35" s="6" t="s">
         <v>22</v>
@@ -1718,7 +1718,7 @@
         <v>-799.4</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="11"/>
       <c r="B36" s="6" t="s">
         <v>23</v>
@@ -1749,7 +1749,7 @@
         <v>-554.84</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="11"/>
       <c r="B37" s="6" t="s">
         <v>24</v>
@@ -1780,7 +1780,7 @@
         <v>-272.39999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="11"/>
       <c r="B38" s="6" t="s">
         <v>25</v>
@@ -1811,37 +1811,62 @@
         <v>-3778.44</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
       <c r="B39" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C39" s="2">
+        <v>471</v>
+      </c>
+      <c r="D39" s="2">
+        <v>931</v>
+      </c>
+      <c r="E39" s="2">
+        <v>86.42</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0</v>
+      </c>
+      <c r="G39" s="2">
+        <v>0</v>
+      </c>
+      <c r="H39" s="2">
+        <v>0</v>
+      </c>
+      <c r="I39" s="2">
+        <v>0</v>
+      </c>
+      <c r="J39" s="2">
+        <f>(H39+I39)-(C39+D39+E39+F39+G39)</f>
+        <v>-1488.42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
       <c r="B40" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="11"/>
       <c r="B41" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="11"/>
       <c r="B42" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="11"/>
       <c r="B43" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="12"/>
       <c r="B44" s="6" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
docs: update sheets for 2023-08
</commit_message>
<xml_diff>
--- a/汽车收入与开支记录.xlsx
+++ b/汽车收入与开支记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\finance\recording\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DDECDF-20FE-46F7-8D8B-F83E29D16383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEC4A78-0DAC-4170-959A-AACB4533726F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="285" windowWidth="29040" windowHeight="15615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -627,7 +627,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J39" sqref="J39"/>
+      <selection pane="bottomLeft" activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1683,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="2">
-        <f>(H34+I34)-(C34+D34+E34+F34+G34)</f>
+        <f t="shared" ref="J34:J40" si="3">(H34+I34)-(C34+D34+E34+F34+G34)</f>
         <v>-2015.5</v>
       </c>
     </row>
@@ -1714,7 +1714,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="2">
-        <f>(H35+I35)-(C35+D35+E35+F35+G35)</f>
+        <f t="shared" si="3"/>
         <v>-799.4</v>
       </c>
     </row>
@@ -1745,7 +1745,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="2">
-        <f>(H36+I36)-(C36+D36+E36+F36+G36)</f>
+        <f t="shared" si="3"/>
         <v>-554.84</v>
       </c>
     </row>
@@ -1776,7 +1776,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="2">
-        <f>(H37+I37)-(C37+D37+E37+F37+G37)</f>
+        <f t="shared" si="3"/>
         <v>-272.39999999999998</v>
       </c>
     </row>
@@ -1807,7 +1807,7 @@
         <v>0</v>
       </c>
       <c r="J38" s="2">
-        <f>(H38+I38)-(C38+D38+E38+F38+G38)</f>
+        <f t="shared" si="3"/>
         <v>-3778.44</v>
       </c>
     </row>
@@ -1838,7 +1838,7 @@
         <v>0</v>
       </c>
       <c r="J39" s="2">
-        <f>(H39+I39)-(C39+D39+E39+F39+G39)</f>
+        <f t="shared" si="3"/>
         <v>-1488.42</v>
       </c>
     </row>
@@ -1846,6 +1846,31 @@
       <c r="A40" s="11"/>
       <c r="B40" s="6" t="s">
         <v>14</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2">
+        <v>826.62</v>
+      </c>
+      <c r="E40" s="2">
+        <v>3</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0</v>
+      </c>
+      <c r="G40" s="2">
+        <v>9.9</v>
+      </c>
+      <c r="H40" s="2">
+        <v>0</v>
+      </c>
+      <c r="I40" s="2">
+        <v>0</v>
+      </c>
+      <c r="J40" s="2">
+        <f t="shared" si="3"/>
+        <v>-839.52</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat: update sheets for 2023-10
</commit_message>
<xml_diff>
--- a/汽车收入与开支记录.xlsx
+++ b/汽车收入与开支记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\finance\recording\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEC4A78-0DAC-4170-959A-AACB4533726F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6423AC8D-F5AC-4C51-ADBF-2CCE9954A550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="285" windowWidth="29040" windowHeight="15615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="300" windowWidth="23256" windowHeight="12348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -626,20 +626,20 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J40" sqref="J40"/>
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="8" width="9" style="2"/>
-    <col min="9" max="9" width="10.5" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.375" style="2"/>
+    <col min="9" max="9" width="10.44140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" style="2"/>
     <col min="11" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -661,7 +661,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
       <c r="B2" s="14"/>
       <c r="C2" s="4" t="s">
@@ -687,7 +687,7 @@
       </c>
       <c r="J2" s="15"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>12</v>
       </c>
@@ -720,7 +720,7 @@
         <v>-732.93000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="21"/>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -751,7 +751,7 @@
         <v>6.2000000000000455</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="21"/>
       <c r="B5" s="1" t="s">
         <v>15</v>
@@ -782,7 +782,7 @@
         <v>-388.07</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
@@ -813,7 +813,7 @@
         <v>-382</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
@@ -844,7 +844,7 @@
         <v>-210</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="1" t="s">
         <v>18</v>
@@ -875,7 +875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>19</v>
       </c>
@@ -908,7 +908,7 @@
         <v>-300</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="1" t="s">
         <v>21</v>
@@ -939,7 +939,7 @@
         <v>-285</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="1" t="s">
         <v>22</v>
@@ -970,7 +970,7 @@
         <v>-1785</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="5" t="s">
         <v>23</v>
@@ -1001,7 +1001,7 @@
         <v>-734.93000000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="B13" s="1" t="s">
         <v>24</v>
@@ -1032,7 +1032,7 @@
         <v>-215.7</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="5" t="s">
         <v>25</v>
@@ -1063,7 +1063,7 @@
         <v>-3986.7400000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="1" t="s">
         <v>13</v>
@@ -1094,7 +1094,7 @@
         <v>-276.89999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
       <c r="B16" s="5" t="s">
         <v>14</v>
@@ -1125,7 +1125,7 @@
         <v>-95.419999999999959</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="1" t="s">
         <v>15</v>
@@ -1156,7 +1156,7 @@
         <v>-278.98</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="21"/>
       <c r="B18" s="5" t="s">
         <v>16</v>
@@ -1187,7 +1187,7 @@
         <v>-11.700000000000045</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
       <c r="B19" s="5" t="s">
         <v>26</v>
@@ -1218,7 +1218,7 @@
         <v>-77.650000000000034</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="5" t="s">
         <v>18</v>
@@ -1249,7 +1249,7 @@
         <v>34.490000000000009</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>27</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>-21.180000000000035</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="5" t="s">
         <v>21</v>
@@ -1313,7 +1313,7 @@
         <v>-221.57</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="5" t="s">
         <v>22</v>
@@ -1344,7 +1344,7 @@
         <v>-59.820000000000022</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="5" t="s">
         <v>23</v>
@@ -1375,7 +1375,7 @@
         <v>-16.080000000000013</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="5" t="s">
         <v>24</v>
@@ -1406,7 +1406,7 @@
         <v>-230</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="5" t="s">
         <v>25</v>
@@ -1437,7 +1437,7 @@
         <v>-3857.52</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="1" t="s">
         <v>13</v>
@@ -1468,7 +1468,7 @@
         <v>-280</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="6" t="s">
         <v>14</v>
@@ -1499,7 +1499,7 @@
         <v>-181.54</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="6" t="s">
         <v>15</v>
@@ -1530,7 +1530,7 @@
         <v>-452.79</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="6" t="s">
         <v>16</v>
@@ -1561,7 +1561,7 @@
         <v>-650.9</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="6" t="s">
         <v>17</v>
@@ -1592,7 +1592,7 @@
         <v>-603.41000000000008</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="6" t="s">
         <v>18</v>
@@ -1623,7 +1623,7 @@
         <v>-894.4</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>28</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>-148</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="6" t="s">
         <v>21</v>
@@ -1683,11 +1683,11 @@
         <v>0</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" ref="J34:J40" si="3">(H34+I34)-(C34+D34+E34+F34+G34)</f>
+        <f t="shared" ref="J34:J42" si="3">(H34+I34)-(C34+D34+E34+F34+G34)</f>
         <v>-2015.5</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="6" t="s">
         <v>22</v>
@@ -1718,7 +1718,7 @@
         <v>-799.4</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="6" t="s">
         <v>23</v>
@@ -1749,7 +1749,7 @@
         <v>-554.84</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="6" t="s">
         <v>24</v>
@@ -1780,7 +1780,7 @@
         <v>-272.39999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="6" t="s">
         <v>25</v>
@@ -1811,7 +1811,7 @@
         <v>-3778.44</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="6" t="s">
         <v>13</v>
@@ -1842,7 +1842,7 @@
         <v>-1488.42</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="6" t="s">
         <v>14</v>
@@ -1873,25 +1873,75 @@
         <v>-839.52</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C41" s="2">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2">
+        <v>351</v>
+      </c>
+      <c r="E41" s="2">
+        <v>31.2</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0</v>
+      </c>
+      <c r="G41" s="2">
+        <v>0</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0</v>
+      </c>
+      <c r="I41" s="2">
+        <v>0</v>
+      </c>
+      <c r="J41" s="2">
+        <f t="shared" si="3"/>
+        <v>-382.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C42" s="2">
+        <v>270</v>
+      </c>
+      <c r="D42" s="2">
+        <v>39</v>
+      </c>
+      <c r="E42" s="2">
+        <v>13.53</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0</v>
+      </c>
+      <c r="G42" s="2">
+        <v>0</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0</v>
+      </c>
+      <c r="I42" s="2">
+        <v>0</v>
+      </c>
+      <c r="J42" s="2">
+        <f t="shared" si="3"/>
+        <v>-322.52999999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="6" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
feat: update sheets for 2023-11
</commit_message>
<xml_diff>
--- a/汽车收入与开支记录.xlsx
+++ b/汽车收入与开支记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\finance\recording\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6423AC8D-F5AC-4C51-ADBF-2CCE9954A550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454103B9-F39B-4338-BC23-1213AED8037C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="300" windowWidth="23256" windowHeight="12348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="285" windowWidth="29040" windowHeight="15615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -627,19 +627,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J42" sqref="J42"/>
+      <selection pane="bottomLeft" activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="8" width="9" style="2"/>
-    <col min="9" max="9" width="10.44140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" style="2"/>
+    <col min="9" max="9" width="10.5" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.375" style="2"/>
     <col min="11" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -661,7 +661,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="19"/>
       <c r="B2" s="14"/>
       <c r="C2" s="4" t="s">
@@ -687,7 +687,7 @@
       </c>
       <c r="J2" s="15"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>12</v>
       </c>
@@ -720,7 +720,7 @@
         <v>-732.93000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="21"/>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -751,7 +751,7 @@
         <v>6.2000000000000455</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="21"/>
       <c r="B5" s="1" t="s">
         <v>15</v>
@@ -782,7 +782,7 @@
         <v>-388.07</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="21"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
@@ -813,7 +813,7 @@
         <v>-382</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="21"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
@@ -844,7 +844,7 @@
         <v>-210</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="22"/>
       <c r="B8" s="1" t="s">
         <v>18</v>
@@ -875,7 +875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
         <v>19</v>
       </c>
@@ -908,7 +908,7 @@
         <v>-300</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="21"/>
       <c r="B10" s="1" t="s">
         <v>21</v>
@@ -939,7 +939,7 @@
         <v>-285</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="21"/>
       <c r="B11" s="1" t="s">
         <v>22</v>
@@ -970,7 +970,7 @@
         <v>-1785</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="21"/>
       <c r="B12" s="5" t="s">
         <v>23</v>
@@ -1001,7 +1001,7 @@
         <v>-734.93000000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="21"/>
       <c r="B13" s="1" t="s">
         <v>24</v>
@@ -1032,7 +1032,7 @@
         <v>-215.7</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="21"/>
       <c r="B14" s="5" t="s">
         <v>25</v>
@@ -1063,7 +1063,7 @@
         <v>-3986.7400000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="21"/>
       <c r="B15" s="1" t="s">
         <v>13</v>
@@ -1094,7 +1094,7 @@
         <v>-276.89999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="21"/>
       <c r="B16" s="5" t="s">
         <v>14</v>
@@ -1125,7 +1125,7 @@
         <v>-95.419999999999959</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="21"/>
       <c r="B17" s="1" t="s">
         <v>15</v>
@@ -1156,7 +1156,7 @@
         <v>-278.98</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="21"/>
       <c r="B18" s="5" t="s">
         <v>16</v>
@@ -1187,7 +1187,7 @@
         <v>-11.700000000000045</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="21"/>
       <c r="B19" s="5" t="s">
         <v>26</v>
@@ -1218,7 +1218,7 @@
         <v>-77.650000000000034</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="22"/>
       <c r="B20" s="5" t="s">
         <v>18</v>
@@ -1249,7 +1249,7 @@
         <v>34.490000000000009</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>27</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>-21.180000000000035</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="5" t="s">
         <v>21</v>
@@ -1313,7 +1313,7 @@
         <v>-221.57</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="5" t="s">
         <v>22</v>
@@ -1344,7 +1344,7 @@
         <v>-59.820000000000022</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="5" t="s">
         <v>23</v>
@@ -1375,7 +1375,7 @@
         <v>-16.080000000000013</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
       <c r="B25" s="5" t="s">
         <v>24</v>
@@ -1406,7 +1406,7 @@
         <v>-230</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="5" t="s">
         <v>25</v>
@@ -1437,7 +1437,7 @@
         <v>-3857.52</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
       <c r="B27" s="1" t="s">
         <v>13</v>
@@ -1468,7 +1468,7 @@
         <v>-280</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="6" t="s">
         <v>14</v>
@@ -1499,7 +1499,7 @@
         <v>-181.54</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
       <c r="B29" s="6" t="s">
         <v>15</v>
@@ -1530,7 +1530,7 @@
         <v>-452.79</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="6" t="s">
         <v>16</v>
@@ -1561,7 +1561,7 @@
         <v>-650.9</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
       <c r="B31" s="6" t="s">
         <v>17</v>
@@ -1592,7 +1592,7 @@
         <v>-603.41000000000008</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
       <c r="B32" s="6" t="s">
         <v>18</v>
@@ -1623,7 +1623,7 @@
         <v>-894.4</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>28</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>-148</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
       <c r="B34" s="6" t="s">
         <v>21</v>
@@ -1683,11 +1683,11 @@
         <v>0</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" ref="J34:J42" si="3">(H34+I34)-(C34+D34+E34+F34+G34)</f>
+        <f t="shared" ref="J34:J43" si="3">(H34+I34)-(C34+D34+E34+F34+G34)</f>
         <v>-2015.5</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
       <c r="B35" s="6" t="s">
         <v>22</v>
@@ -1718,7 +1718,7 @@
         <v>-799.4</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="11"/>
       <c r="B36" s="6" t="s">
         <v>23</v>
@@ -1749,7 +1749,7 @@
         <v>-554.84</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="11"/>
       <c r="B37" s="6" t="s">
         <v>24</v>
@@ -1780,7 +1780,7 @@
         <v>-272.39999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="11"/>
       <c r="B38" s="6" t="s">
         <v>25</v>
@@ -1811,7 +1811,7 @@
         <v>-3778.44</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
       <c r="B39" s="6" t="s">
         <v>13</v>
@@ -1842,7 +1842,7 @@
         <v>-1488.42</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
       <c r="B40" s="6" t="s">
         <v>14</v>
@@ -1873,7 +1873,7 @@
         <v>-839.52</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="11"/>
       <c r="B41" s="6" t="s">
         <v>15</v>
@@ -1904,7 +1904,7 @@
         <v>-382.2</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="11"/>
       <c r="B42" s="6" t="s">
         <v>16</v>
@@ -1935,13 +1935,38 @@
         <v>-322.52999999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="11"/>
       <c r="B43" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C43" s="2">
+        <v>1027.29</v>
+      </c>
+      <c r="D43" s="2">
+        <v>593</v>
+      </c>
+      <c r="E43" s="2">
+        <v>55</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0</v>
+      </c>
+      <c r="G43" s="2">
+        <v>0</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0</v>
+      </c>
+      <c r="I43" s="2">
+        <v>0</v>
+      </c>
+      <c r="J43" s="2">
+        <f t="shared" si="3"/>
+        <v>-1675.29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="12"/>
       <c r="B44" s="6" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
feat: update sheets for 2023-12
</commit_message>
<xml_diff>
--- a/汽车收入与开支记录.xlsx
+++ b/汽车收入与开支记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\finance\recording\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454103B9-F39B-4338-BC23-1213AED8037C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BF2E4B-3467-46DD-B059-1F1D5D5BF99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="285" windowWidth="29040" windowHeight="15615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -627,7 +627,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J43" sqref="J43"/>
+      <selection pane="bottomLeft" activeCell="N49" sqref="N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1683,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" ref="J34:J43" si="3">(H34+I34)-(C34+D34+E34+F34+G34)</f>
+        <f t="shared" ref="J34:J44" si="3">(H34+I34)-(C34+D34+E34+F34+G34)</f>
         <v>-2015.5</v>
       </c>
     </row>
@@ -1970,6 +1970,31 @@
       <c r="A44" s="12"/>
       <c r="B44" s="6" t="s">
         <v>18</v>
+      </c>
+      <c r="C44" s="2">
+        <v>1110.01</v>
+      </c>
+      <c r="D44" s="2">
+        <v>380</v>
+      </c>
+      <c r="E44" s="2">
+        <v>173.9</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0</v>
+      </c>
+      <c r="G44" s="2">
+        <v>359.99</v>
+      </c>
+      <c r="H44" s="2">
+        <v>0</v>
+      </c>
+      <c r="I44" s="2">
+        <v>0</v>
+      </c>
+      <c r="J44" s="2">
+        <f t="shared" si="3"/>
+        <v>-2023.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: update sheets for 2024-01
</commit_message>
<xml_diff>
--- a/汽车收入与开支记录.xlsx
+++ b/汽车收入与开支记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\finance\recording\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BF2E4B-3467-46DD-B059-1F1D5D5BF99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B89C42F-3CEF-4155-A839-0AAD02991760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="285" windowWidth="29040" windowHeight="15615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="31">
   <si>
     <t>年份</t>
   </si>
@@ -138,12 +138,20 @@
   <si>
     <t>2023</t>
   </si>
+  <si>
+    <t>2024</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +169,14 @@
     <font>
       <sz val="9"/>
       <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -280,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -346,6 +362,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -623,11 +645,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N49" sqref="N49"/>
+      <selection pane="bottomLeft" activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1683,7 +1705,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" ref="J34:J44" si="3">(H34+I34)-(C34+D34+E34+F34+G34)</f>
+        <f t="shared" ref="J34:J45" si="3">(H34+I34)-(C34+D34+E34+F34+G34)</f>
         <v>-2015.5</v>
       </c>
     </row>
@@ -1997,8 +2019,108 @@
         <v>-2023.9</v>
       </c>
     </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B45" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45" s="2">
+        <v>297.26</v>
+      </c>
+      <c r="D45" s="2">
+        <v>1032</v>
+      </c>
+      <c r="E45" s="2">
+        <v>105.5</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0</v>
+      </c>
+      <c r="G45" s="2">
+        <v>0</v>
+      </c>
+      <c r="H45" s="2">
+        <v>0</v>
+      </c>
+      <c r="I45" s="2">
+        <v>0</v>
+      </c>
+      <c r="J45" s="2">
+        <f t="shared" si="3"/>
+        <v>-1434.76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="21"/>
+      <c r="B46" s="24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="21"/>
+      <c r="B47" s="24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="21"/>
+      <c r="B48" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="21"/>
+      <c r="B49" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="21"/>
+      <c r="B50" s="24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="21"/>
+      <c r="B51" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="21"/>
+      <c r="B52" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="21"/>
+      <c r="B53" s="24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="21"/>
+      <c r="B54" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="21"/>
+      <c r="B55" s="24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="22"/>
+      <c r="B56" s="24" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="A45:A56"/>
     <mergeCell ref="A21:A32"/>
     <mergeCell ref="A33:A44"/>
     <mergeCell ref="B1:B2"/>

</xml_diff>

<commit_message>
feat: update sheets for 2024-03
</commit_message>
<xml_diff>
--- a/汽车收入与开支记录.xlsx
+++ b/汽车收入与开支记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\finance\recording\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B89C42F-3CEF-4155-A839-0AAD02991760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4E0903-5B21-4BA0-BDBA-89AA442420EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="285" windowWidth="29040" windowHeight="15615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -316,6 +316,18 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -356,18 +368,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -649,7 +649,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J45" sqref="J45"/>
+      <selection pane="bottomLeft" activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -662,30 +662,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13" t="s">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="16" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="15" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="19" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="14"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
@@ -707,10 +707,10 @@
       <c r="I2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="15"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="24" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -743,7 +743,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="21"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
@@ -774,7 +774,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="21"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
@@ -805,7 +805,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="21"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
@@ -836,7 +836,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
@@ -867,7 +867,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="22"/>
+      <c r="A8" s="10"/>
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
@@ -898,7 +898,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -931,7 +931,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="21"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
@@ -962,7 +962,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="21"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
@@ -993,7 +993,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="5" t="s">
         <v>23</v>
       </c>
@@ -1024,7 +1024,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="21"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
@@ -1055,7 +1055,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="21"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
@@ -1086,7 +1086,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="21"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1117,7 +1117,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="21"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="5" t="s">
         <v>14</v>
       </c>
@@ -1148,7 +1148,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="21"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1179,7 +1179,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="21"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="5" t="s">
         <v>16</v>
       </c>
@@ -1210,7 +1210,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="21"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="5" t="s">
         <v>26</v>
       </c>
@@ -1241,7 +1241,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="22"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="5" t="s">
         <v>18</v>
       </c>
@@ -1272,7 +1272,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -1305,7 +1305,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="5" t="s">
         <v>21</v>
       </c>
@@ -1336,7 +1336,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="8"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="5" t="s">
         <v>22</v>
       </c>
@@ -1367,7 +1367,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="5" t="s">
         <v>23</v>
       </c>
@@ -1398,7 +1398,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="8"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="5" t="s">
         <v>24</v>
       </c>
@@ -1429,7 +1429,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="5" t="s">
         <v>25</v>
       </c>
@@ -1460,7 +1460,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="8"/>
+      <c r="A27" s="12"/>
       <c r="B27" s="1" t="s">
         <v>13</v>
       </c>
@@ -1491,7 +1491,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
+      <c r="A28" s="12"/>
       <c r="B28" s="6" t="s">
         <v>14</v>
       </c>
@@ -1522,7 +1522,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="8"/>
+      <c r="A29" s="12"/>
       <c r="B29" s="6" t="s">
         <v>15</v>
       </c>
@@ -1553,7 +1553,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="8"/>
+      <c r="A30" s="12"/>
       <c r="B30" s="6" t="s">
         <v>16</v>
       </c>
@@ -1584,7 +1584,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="8"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="6" t="s">
         <v>17</v>
       </c>
@@ -1615,7 +1615,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
+      <c r="A32" s="13"/>
       <c r="B32" s="6" t="s">
         <v>18</v>
       </c>
@@ -1646,7 +1646,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B33" s="6" t="s">
@@ -1679,7 +1679,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="11"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="6" t="s">
         <v>21</v>
       </c>
@@ -1705,12 +1705,12 @@
         <v>0</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" ref="J34:J45" si="3">(H34+I34)-(C34+D34+E34+F34+G34)</f>
+        <f t="shared" ref="J34:J47" si="3">(H34+I34)-(C34+D34+E34+F34+G34)</f>
         <v>-2015.5</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="11"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="6" t="s">
         <v>22</v>
       </c>
@@ -1741,7 +1741,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="11"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="6" t="s">
         <v>23</v>
       </c>
@@ -1772,7 +1772,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="11"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="6" t="s">
         <v>24</v>
       </c>
@@ -1803,7 +1803,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="11"/>
+      <c r="A38" s="15"/>
       <c r="B38" s="6" t="s">
         <v>25</v>
       </c>
@@ -1834,7 +1834,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="11"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="6" t="s">
         <v>13</v>
       </c>
@@ -1865,7 +1865,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="11"/>
+      <c r="A40" s="15"/>
       <c r="B40" s="6" t="s">
         <v>14</v>
       </c>
@@ -1896,7 +1896,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="11"/>
+      <c r="A41" s="15"/>
       <c r="B41" s="6" t="s">
         <v>15</v>
       </c>
@@ -1927,7 +1927,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42" s="11"/>
+      <c r="A42" s="15"/>
       <c r="B42" s="6" t="s">
         <v>16</v>
       </c>
@@ -1958,7 +1958,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" s="11"/>
+      <c r="A43" s="15"/>
       <c r="B43" s="6" t="s">
         <v>17</v>
       </c>
@@ -1989,7 +1989,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="12"/>
+      <c r="A44" s="16"/>
       <c r="B44" s="6" t="s">
         <v>18</v>
       </c>
@@ -2020,10 +2020,10 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B45" s="24" t="s">
+      <c r="B45" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C45" s="2">
@@ -2053,68 +2053,118 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" s="21"/>
-      <c r="B46" s="24" t="s">
+      <c r="A46" s="9"/>
+      <c r="B46" s="7" t="s">
         <v>21</v>
       </c>
+      <c r="C46" s="2">
+        <v>279.14</v>
+      </c>
+      <c r="D46" s="2">
+        <v>185</v>
+      </c>
+      <c r="E46" s="2">
+        <v>0</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0</v>
+      </c>
+      <c r="G46" s="2">
+        <v>0</v>
+      </c>
+      <c r="H46" s="2">
+        <v>0</v>
+      </c>
+      <c r="I46" s="2">
+        <v>0</v>
+      </c>
+      <c r="J46" s="2">
+        <f t="shared" si="3"/>
+        <v>-464.14</v>
+      </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="21"/>
-      <c r="B47" s="24" t="s">
+      <c r="A47" s="9"/>
+      <c r="B47" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="C47" s="2">
+        <v>450</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0</v>
+      </c>
+      <c r="E47" s="2">
+        <v>17.7</v>
+      </c>
+      <c r="F47" s="2">
+        <v>0</v>
+      </c>
+      <c r="G47" s="2">
+        <v>0</v>
+      </c>
+      <c r="H47" s="2">
+        <v>0</v>
+      </c>
+      <c r="I47" s="2">
+        <v>0</v>
+      </c>
+      <c r="J47" s="2">
+        <f t="shared" si="3"/>
+        <v>-467.7</v>
+      </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="21"/>
-      <c r="B48" s="24" t="s">
+      <c r="A48" s="9"/>
+      <c r="B48" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="21"/>
-      <c r="B49" s="24" t="s">
+      <c r="A49" s="9"/>
+      <c r="B49" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="21"/>
-      <c r="B50" s="24" t="s">
+      <c r="A50" s="9"/>
+      <c r="B50" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="21"/>
-      <c r="B51" s="24" t="s">
+      <c r="A51" s="9"/>
+      <c r="B51" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="21"/>
-      <c r="B52" s="24" t="s">
+      <c r="A52" s="9"/>
+      <c r="B52" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="21"/>
-      <c r="B53" s="24" t="s">
+      <c r="A53" s="9"/>
+      <c r="B53" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="21"/>
-      <c r="B54" s="24" t="s">
+      <c r="A54" s="9"/>
+      <c r="B54" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="21"/>
-      <c r="B55" s="24" t="s">
+      <c r="A55" s="9"/>
+      <c r="B55" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="22"/>
-      <c r="B56" s="24" t="s">
+      <c r="A56" s="10"/>
+      <c r="B56" s="7" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: update sheets for 2024-04
</commit_message>
<xml_diff>
--- a/汽车收入与开支记录.xlsx
+++ b/汽车收入与开支记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\finance\recording\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4E0903-5B21-4BA0-BDBA-89AA442420EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABED692F-B94B-4957-9889-0CAEDAF4A0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="285" windowWidth="29040" windowHeight="15615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -649,7 +649,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J47" sqref="J47"/>
+      <selection pane="bottomLeft" activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1705,7 +1705,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" ref="J34:J47" si="3">(H34+I34)-(C34+D34+E34+F34+G34)</f>
+        <f t="shared" ref="J34:J48" si="3">(H34+I34)-(C34+D34+E34+F34+G34)</f>
         <v>-2015.5</v>
       </c>
     </row>
@@ -2118,6 +2118,31 @@
       <c r="A48" s="9"/>
       <c r="B48" s="7" t="s">
         <v>23</v>
+      </c>
+      <c r="C48" s="2">
+        <v>768</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0</v>
+      </c>
+      <c r="E48" s="2">
+        <v>22</v>
+      </c>
+      <c r="F48" s="2">
+        <v>0</v>
+      </c>
+      <c r="G48" s="2">
+        <v>300</v>
+      </c>
+      <c r="H48" s="2">
+        <v>0</v>
+      </c>
+      <c r="I48" s="2">
+        <v>0</v>
+      </c>
+      <c r="J48" s="2">
+        <f t="shared" si="3"/>
+        <v>-1090</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat: update sheets for 2024-06
</commit_message>
<xml_diff>
--- a/汽车收入与开支记录.xlsx
+++ b/汽车收入与开支记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\finance\recording\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABED692F-B94B-4957-9889-0CAEDAF4A0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD0CB35-ADB9-457C-AB6C-6718F25E4F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="285" windowWidth="29040" windowHeight="15615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="300" windowWidth="23256" windowHeight="12348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -648,20 +648,20 @@
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J48" sqref="J48"/>
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="8" width="9" style="2"/>
-    <col min="9" max="9" width="10.5" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.375" style="2"/>
+    <col min="9" max="9" width="10.44140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" style="2"/>
     <col min="11" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -683,7 +683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="23"/>
       <c r="B2" s="18"/>
       <c r="C2" s="4" t="s">
@@ -709,7 +709,7 @@
       </c>
       <c r="J2" s="19"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>12</v>
       </c>
@@ -742,7 +742,7 @@
         <v>-732.93000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -773,7 +773,7 @@
         <v>6.2000000000000455</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="1" t="s">
         <v>15</v>
@@ -804,7 +804,7 @@
         <v>-388.07</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
@@ -835,7 +835,7 @@
         <v>-382</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
@@ -866,7 +866,7 @@
         <v>-210</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="1" t="s">
         <v>18</v>
@@ -897,7 +897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>19</v>
       </c>
@@ -930,7 +930,7 @@
         <v>-300</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="1" t="s">
         <v>21</v>
@@ -961,7 +961,7 @@
         <v>-285</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="1" t="s">
         <v>22</v>
@@ -992,7 +992,7 @@
         <v>-1785</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="5" t="s">
         <v>23</v>
@@ -1023,7 +1023,7 @@
         <v>-734.93000000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="1" t="s">
         <v>24</v>
@@ -1054,7 +1054,7 @@
         <v>-215.7</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="5" t="s">
         <v>25</v>
@@ -1085,7 +1085,7 @@
         <v>-3986.7400000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="1" t="s">
         <v>13</v>
@@ -1116,7 +1116,7 @@
         <v>-276.89999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="5" t="s">
         <v>14</v>
@@ -1147,7 +1147,7 @@
         <v>-95.419999999999959</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="1" t="s">
         <v>15</v>
@@ -1178,7 +1178,7 @@
         <v>-278.98</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="5" t="s">
         <v>16</v>
@@ -1209,7 +1209,7 @@
         <v>-11.700000000000045</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="5" t="s">
         <v>26</v>
@@ -1240,7 +1240,7 @@
         <v>-77.650000000000034</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="5" t="s">
         <v>18</v>
@@ -1271,7 +1271,7 @@
         <v>34.490000000000009</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>27</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>-21.180000000000035</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="5" t="s">
         <v>21</v>
@@ -1335,7 +1335,7 @@
         <v>-221.57</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="5" t="s">
         <v>22</v>
@@ -1366,7 +1366,7 @@
         <v>-59.820000000000022</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="5" t="s">
         <v>23</v>
@@ -1397,7 +1397,7 @@
         <v>-16.080000000000013</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="5" t="s">
         <v>24</v>
@@ -1428,7 +1428,7 @@
         <v>-230</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="5" t="s">
         <v>25</v>
@@ -1459,7 +1459,7 @@
         <v>-3857.52</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="1" t="s">
         <v>13</v>
@@ -1490,7 +1490,7 @@
         <v>-280</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="6" t="s">
         <v>14</v>
@@ -1521,7 +1521,7 @@
         <v>-181.54</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="6" t="s">
         <v>15</v>
@@ -1552,7 +1552,7 @@
         <v>-452.79</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="6" t="s">
         <v>16</v>
@@ -1583,7 +1583,7 @@
         <v>-650.9</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="6" t="s">
         <v>17</v>
@@ -1614,7 +1614,7 @@
         <v>-603.41000000000008</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="6" t="s">
         <v>18</v>
@@ -1645,7 +1645,7 @@
         <v>-894.4</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>28</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>-148</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
       <c r="B34" s="6" t="s">
         <v>21</v>
@@ -1705,11 +1705,11 @@
         <v>0</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" ref="J34:J48" si="3">(H34+I34)-(C34+D34+E34+F34+G34)</f>
+        <f t="shared" ref="J34:J50" si="3">(H34+I34)-(C34+D34+E34+F34+G34)</f>
         <v>-2015.5</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
       <c r="B35" s="6" t="s">
         <v>22</v>
@@ -1740,7 +1740,7 @@
         <v>-799.4</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
       <c r="B36" s="6" t="s">
         <v>23</v>
@@ -1771,7 +1771,7 @@
         <v>-554.84</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
       <c r="B37" s="6" t="s">
         <v>24</v>
@@ -1802,7 +1802,7 @@
         <v>-272.39999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
       <c r="B38" s="6" t="s">
         <v>25</v>
@@ -1833,7 +1833,7 @@
         <v>-3778.44</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" s="6" t="s">
         <v>13</v>
@@ -1864,7 +1864,7 @@
         <v>-1488.42</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
       <c r="B40" s="6" t="s">
         <v>14</v>
@@ -1895,7 +1895,7 @@
         <v>-839.52</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
       <c r="B41" s="6" t="s">
         <v>15</v>
@@ -1926,7 +1926,7 @@
         <v>-382.2</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>
       <c r="B42" s="6" t="s">
         <v>16</v>
@@ -1957,7 +1957,7 @@
         <v>-322.52999999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
       <c r="B43" s="6" t="s">
         <v>17</v>
@@ -1988,7 +1988,7 @@
         <v>-1675.29</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
       <c r="B44" s="6" t="s">
         <v>18</v>
@@ -2019,7 +2019,7 @@
         <v>-2023.9</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>29</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>-1434.76</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
       <c r="B46" s="7" t="s">
         <v>21</v>
@@ -2083,7 +2083,7 @@
         <v>-464.14</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
       <c r="B47" s="7" t="s">
         <v>22</v>
@@ -2114,7 +2114,7 @@
         <v>-467.7</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
       <c r="B48" s="7" t="s">
         <v>23</v>
@@ -2145,49 +2145,99 @@
         <v>-1090</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
       <c r="B49" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49" s="2">
+        <v>1</v>
+      </c>
+      <c r="D49" s="2">
+        <v>299</v>
+      </c>
+      <c r="E49" s="2">
+        <v>18</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0</v>
+      </c>
+      <c r="G49" s="2">
+        <v>0</v>
+      </c>
+      <c r="H49" s="2">
+        <v>0</v>
+      </c>
+      <c r="I49" s="2">
+        <v>0</v>
+      </c>
+      <c r="J49" s="2">
+        <f t="shared" si="3"/>
+        <v>-318</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="9"/>
       <c r="B50" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50" s="2">
+        <v>781</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0</v>
+      </c>
+      <c r="E50" s="2">
+        <v>10</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0</v>
+      </c>
+      <c r="G50" s="2">
+        <v>3678.39</v>
+      </c>
+      <c r="H50" s="2">
+        <v>0</v>
+      </c>
+      <c r="I50" s="2">
+        <v>0</v>
+      </c>
+      <c r="J50" s="2">
+        <f t="shared" si="3"/>
+        <v>-4469.3899999999994</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="9"/>
       <c r="B51" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
       <c r="B52" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
       <c r="B53" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
       <c r="B54" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="9"/>
       <c r="B55" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="B56" s="7" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
feat: update sheets for 2024-07
</commit_message>
<xml_diff>
--- a/汽车收入与开支记录.xlsx
+++ b/汽车收入与开支记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\finance\recording\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD0CB35-ADB9-457C-AB6C-6718F25E4F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAD6BB0-C0A2-4FBF-952B-9C79E9285AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="300" windowWidth="23256" windowHeight="12348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -649,7 +649,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J50" sqref="J50"/>
+      <selection pane="bottomLeft" activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1705,7 +1705,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" ref="J34:J50" si="3">(H34+I34)-(C34+D34+E34+F34+G34)</f>
+        <f t="shared" ref="J34:J51" si="3">(H34+I34)-(C34+D34+E34+F34+G34)</f>
         <v>-2015.5</v>
       </c>
     </row>
@@ -2211,6 +2211,31 @@
       <c r="A51" s="9"/>
       <c r="B51" s="7" t="s">
         <v>13</v>
+      </c>
+      <c r="C51" s="2">
+        <v>703</v>
+      </c>
+      <c r="D51" s="2">
+        <v>183</v>
+      </c>
+      <c r="E51" s="2">
+        <v>10</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0</v>
+      </c>
+      <c r="G51" s="2">
+        <v>3365</v>
+      </c>
+      <c r="H51" s="2">
+        <v>0</v>
+      </c>
+      <c r="I51" s="2">
+        <v>0</v>
+      </c>
+      <c r="J51" s="2">
+        <f t="shared" si="3"/>
+        <v>-4261</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>